<commit_message>
v2.0.0 需要测试 ASCII To HEX
</commit_message>
<xml_diff>
--- a/MQTT采集终端/MQTT采集器程序(新加 MQTT MBUS 网口功能)/Interflow/AT指令集_MQTT_ED2.xlsx
+++ b/MQTT采集终端/MQTT采集器程序(新加 MQTT MBUS 网口功能)/Interflow/AT指令集_MQTT_ED2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\临时文件夹\WorkSpace\MQTT采集终端\MQTT采集器程序(新加 MQTT MBUS 网口功能)\Interflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C9FDC2-B891-4F7E-BD76-6E7D6861205B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA76E3D-6A73-4561-A6E0-D020B51D44EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AT指令表" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="300">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,9 +133,6 @@
     <t>//恢复模块设置为默认参数</t>
   </si>
   <si>
-    <t>//从出厂参数区恢复参数</t>
-  </si>
-  <si>
     <t>//查询模块固件版本</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
     <t>AT+MQTTLWTCFG==/will,0,ON,offline</t>
   </si>
   <si>
-    <t>AT+MQTTPUBCUSEN=ON</t>
-  </si>
-  <si>
     <t>AT+MQTTHEARTTM=60</t>
   </si>
   <si>
@@ -680,130 +674,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>退出AT命令模式，进入透传模式=0</t>
-  </si>
-  <si>
-    <t>进入ATCmd模式=0</t>
-  </si>
-  <si>
     <t>+++</t>
   </si>
   <si>
-    <t>确认进入AT模式=0</t>
-  </si>
-  <si>
-    <t>查询模块固件版本=0</t>
-  </si>
-  <si>
-    <t>回显使能=0</t>
-  </si>
-  <si>
-    <t>N号串口接口参数=0</t>
-  </si>
-  <si>
     <t>AT+UART2=115200,8,1,NONE,NFC</t>
   </si>
   <si>
-    <t>连接前是否清理串口缓存=0</t>
-  </si>
-  <si>
-    <t>模块DNS获取方式=0</t>
-  </si>
-  <si>
     <t>AT+DNSTYPE=AUTO</t>
   </si>
   <si>
-    <t>模块获取到的WAN口IP（DHCP/STATIC）=0</t>
-  </si>
-  <si>
     <t>AT+WANN=STATIC,192.168.1.117,255.255.255.0,192.168.1.1</t>
   </si>
   <si>
-    <t>WebSocket端口号=0</t>
-  </si>
-  <si>
     <t>AT+WEBSOCKPORT1=6432</t>
   </si>
   <si>
-    <t>N号串口的最大连接数量=0</t>
-  </si>
-  <si>
     <t>AT+MAXSK2=1</t>
   </si>
   <si>
-    <t>N号串口的TCPS超过最大连接数的工作模式=0</t>
-  </si>
-  <si>
     <t>AT+TCPSE2=KICK</t>
   </si>
   <si>
-    <t>N号串口的socket状态（M参数为socket号）=0</t>
-  </si>
-  <si>
-    <t>AT+SOCKA2=TCPC,59.110.170.225,1883</t>
-  </si>
-  <si>
-    <t>查询N号串口的socketM的连接状态=0</t>
-  </si>
-  <si>
-    <t>MQTT网关功能状态=0</t>
-  </si>
-  <si>
-    <t>MQTTsocket连接本地端口号=0</t>
-  </si>
-  <si>
     <t>AT+MQTTLPORT=0</t>
   </si>
   <si>
-    <t>MQTT连接验证开启状态=0</t>
-  </si>
-  <si>
-    <t>MQTT客户端ID=0</t>
-  </si>
-  <si>
-    <t>AT+MQTTCID=HY_ql</t>
-  </si>
-  <si>
-    <t>MQTT用户名=0</t>
-  </si>
-  <si>
     <t>AT+MQTTUSER=ql</t>
   </si>
   <si>
-    <t>MQTT用户密码=0</t>
-  </si>
-  <si>
     <t>AT+MQTTPSW=ql</t>
-  </si>
-  <si>
-    <t>MQTT主题发布自定义模式=0</t>
-  </si>
-  <si>
-    <t>MQTT的预置发布主题信息=0</t>
-  </si>
-  <si>
-    <t>AT+MQTTPUB=1,OFF,/hy/gw/02345678903,0,1,0,OFF,2</t>
-  </si>
-  <si>
-    <t>MQTT的预置订阅主题信息=0</t>
-  </si>
-  <si>
-    <t>AT+MQTTSUB=1,ON,/hy/gw,0,0,&amp;#44,2</t>
-  </si>
-  <si>
-    <t>MQTT网关功能的服务器IP地址，端口号=0</t>
-  </si>
-  <si>
-    <t>模块名称=0</t>
-  </si>
-  <si>
-    <t>WebSocket的方向=0</t>
-  </si>
-  <si>
-    <t>将当前参数保存为用户默认参数=0</t>
-  </si>
-  <si>
-    <t>设备重启=0</t>
   </si>
   <si>
     <t>|0</t>
@@ -934,48 +832,6 @@
     <t>|20|</t>
   </si>
   <si>
-    <t>|21</t>
-  </si>
-  <si>
-    <t>|21|</t>
-  </si>
-  <si>
-    <t>|22</t>
-  </si>
-  <si>
-    <t>|22|</t>
-  </si>
-  <si>
-    <t>|23</t>
-  </si>
-  <si>
-    <t>|23|</t>
-  </si>
-  <si>
-    <t>|24</t>
-  </si>
-  <si>
-    <t>|24|</t>
-  </si>
-  <si>
-    <t>|25</t>
-  </si>
-  <si>
-    <t>|25|</t>
-  </si>
-  <si>
-    <t>|26</t>
-  </si>
-  <si>
-    <t>|26|</t>
-  </si>
-  <si>
-    <t>|27</t>
-  </si>
-  <si>
-    <t>|27|</t>
-  </si>
-  <si>
     <t>AT+MQTTCID=HY_QL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -992,17 +848,6 @@
     <t>setUserAndPassWordDataLoadFun</t>
   </si>
   <si>
-    <t>AT+MQTTSUB=1,ON,/hy/gw/#,0,0,&amp;#44,2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AT+MQTTPUB=1,ON,hy/gw/get/02345678903,0,MY_PUB,0,OFF,2</t>
-  </si>
-  <si>
-    <t>AT+MQTTPUB=1,ON,hy/gw/get/02345678903,0,MY_PUB,0,OFF,2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AT+SOCKLKA2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1038,6 +883,106 @@
   </si>
   <si>
     <t>setMQTTMassageSUBFun</t>
+  </si>
+  <si>
+    <t>//恢复出场参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回显使能</t>
+  </si>
+  <si>
+    <t>N号串口接口参数</t>
+  </si>
+  <si>
+    <t>连接前是否清理串口缓存</t>
+  </si>
+  <si>
+    <t>模块DNS获取方式</t>
+  </si>
+  <si>
+    <t>模块获取到的WAN口IP（DHCP/STATIC）</t>
+  </si>
+  <si>
+    <t>N号串口的最大连接数量</t>
+  </si>
+  <si>
+    <t>MQTT网关功能状态</t>
+  </si>
+  <si>
+    <t>MQTTsocket连接本地端口号</t>
+  </si>
+  <si>
+    <t>MQTT连接验证开启状态</t>
+  </si>
+  <si>
+    <t>MQTT客户端ID</t>
+  </si>
+  <si>
+    <t>MQTT用户名</t>
+  </si>
+  <si>
+    <t>MQTT用户密码</t>
+  </si>
+  <si>
+    <t>MQTT主题发布自定义模式</t>
+  </si>
+  <si>
+    <t>MQTT的预置发布主题信息</t>
+  </si>
+  <si>
+    <t>MQTT的预置订阅主题信息</t>
+  </si>
+  <si>
+    <t>MQTT网关功能的服务器IP地址，端口号</t>
+  </si>
+  <si>
+    <t>设备重启</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>退出AT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTPUBCUSEN=OFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唤醒AT模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入AT模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTEN=ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTLPORT=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTAUTH=ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTPUB=1,ON,hy/gw/set/02345678903,0,MY_PUB,0,OFF,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT+MQTTSUB=1,ON,hy/gw/get/02345678903,0,0,&amp;#44,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1084,7 +1029,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1100,12 +1045,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1139,7 +1078,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1178,7 +1117,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1464,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H29"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A45" sqref="A44:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1513,7 +1453,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
@@ -1531,10 +1471,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I2" s="4" t="str">
         <f>VLOOKUP(MID(IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""""","""""",""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""))),2,LEN(IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""="""""","""""",""""&amp;IF(H2&lt;&gt;"",H2,"")&amp;""""))))-2),A:G,7,0)</f>
@@ -1543,10 +1483,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -1561,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I3" s="4" t="str">
         <f t="shared" ref="I3:I66" si="0">VLOOKUP(MID(IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""""","""""",""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""))),2,LEN(IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""="""""","""""",""""&amp;IF(H3&lt;&gt;"",H3,"")&amp;""""))))-2),A:G,7,0)</f>
@@ -1573,10 +1513,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>21</v>
@@ -1594,7 +1534,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1603,10 +1543,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>21</v>
@@ -1624,7 +1564,7 @@
         <v>24</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1633,10 +1573,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>21</v>
@@ -1651,10 +1591,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1663,10 +1603,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>21</v>
@@ -1681,28 +1621,28 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置WebSocket端口号</v>
+        <v>//查询/设置N号串口的最大连接数量</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1711,22 +1651,22 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置N号串口的最大连接数量</v>
+        <v>//查询/设置MQTT网关功能状态</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>21</v>
@@ -1741,22 +1681,22 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置N号串口的TCPS超过最大连接数的工作模式</v>
+        <v>//查询/设置MQTTsocket连接本地端口号</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>21</v>
@@ -1771,22 +1711,22 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置N号串口的socket状态（M参数为socket号）</v>
+        <v>//查询/设置MQTT连接验证开启状态</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>21</v>
@@ -1801,52 +1741,52 @@
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>312</v>
+        <v>256</v>
       </c>
       <c r="I11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询N号串口的socketM的连接状态</v>
+        <v>//查询/设置MQTT客户端ID</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>314</v>
+      <c r="A12" s="10" t="s">
+        <v>263</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>313</v>
+        <v>262</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>315</v>
+        <v>264</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="I12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置MQTT网关功能状态</v>
+        <v>//查询/设置MQTT用户名</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>21</v>
@@ -1861,22 +1801,22 @@
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="I13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置MQTTsocket连接本地端口号</v>
+        <v>//查询/设置MQTT用户密码</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>21</v>
@@ -1891,22 +1831,22 @@
         <v>1</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>137</v>
+        <v>292</v>
       </c>
       <c r="I14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置MQTT连接验证开启状态</v>
+        <v>//查询/设置MQTT主题发布自定义模式</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>21</v>
@@ -1921,22 +1861,22 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>304</v>
+        <v>93</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="I15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>//查询/设置MQTT客户端ID</v>
+        <v>//查询/设置MQTT的预置发布主题信息</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>21</v>
@@ -1951,142 +1891,138 @@
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="I16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>//查询/设置MQTT的预置订阅主题信息</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT用户名</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT用户密码</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>//设备重启</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT主题发布自定义模式</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="I19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT的预置发布主题信息</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="I20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT的预置订阅主题信息</v>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>21</v>
@@ -2101,22 +2037,20 @@
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I21" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
+        <v>102</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>21</v>
@@ -2131,22 +2065,20 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置模块名称</v>
+        <v>103</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>21</v>
@@ -2161,22 +2093,20 @@
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//查询/设置WebSocket的方向</v>
+        <v>104</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>21</v>
@@ -2191,22 +2121,20 @@
         <v>1</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//设置将当前参数保存为用户默认参数</v>
+        <v>105</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>21</v>
@@ -2221,22 +2149,20 @@
         <v>1</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>//设备重启</v>
+        <v>106</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>21</v>
@@ -2251,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="4" t="e">
@@ -2261,10 +2187,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>21</v>
@@ -2279,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="4" t="e">
@@ -2289,10 +2215,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>135</v>
+        <v>295</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>21</v>
@@ -2307,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="4" t="e">
@@ -2317,10 +2243,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>21</v>
@@ -2335,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="4" t="e">
@@ -2345,10 +2271,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>21</v>
@@ -2363,9 +2289,9 @@
         <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="H30" s="6"/>
       <c r="I30" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2373,16 +2299,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>319</v>
+        <v>268</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
@@ -2391,9 +2317,9 @@
         <v>1</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="13"/>
+        <v>35</v>
+      </c>
+      <c r="H31" s="6"/>
       <c r="I31" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2401,10 +2327,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>230</v>
+        <v>296</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>21</v>
@@ -2419,9 +2345,9 @@
         <v>1</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H32" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="H32" s="6"/>
       <c r="I32" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2429,10 +2355,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>21</v>
@@ -2447,9 +2373,9 @@
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H33" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="H33" s="6"/>
       <c r="I33" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2457,10 +2383,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>21</v>
@@ -2475,9 +2401,9 @@
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2485,10 +2411,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>21</v>
@@ -2503,9 +2429,9 @@
         <v>1</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="H35" s="4"/>
       <c r="I35" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2513,10 +2439,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>21</v>
@@ -2531,9 +2457,9 @@
         <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="H36" s="6"/>
       <c r="I36" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2541,10 +2467,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>137</v>
+        <v>297</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>21</v>
@@ -2559,9 +2485,9 @@
         <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H37" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="H37" s="6"/>
       <c r="I37" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2569,16 +2495,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>316</v>
+        <v>265</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>11</v>
@@ -2587,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="4" t="e">
@@ -2597,16 +2523,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>317</v>
+        <v>266</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>11</v>
@@ -2615,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="4" t="e">
@@ -2625,10 +2551,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>21</v>
@@ -2643,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="4" t="e">
@@ -2653,10 +2579,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>21</v>
@@ -2671,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="4" t="e">
@@ -2681,10 +2607,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>21</v>
@@ -2699,7 +2625,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="4" t="e">
@@ -2709,10 +2635,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>141</v>
+        <v>292</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>21</v>
@@ -2727,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="4" t="e">
@@ -2736,17 +2662,17 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
-        <v>311</v>
+      <c r="A44" s="10" t="s">
+        <v>298</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>11</v>
@@ -2755,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="4" t="e">
@@ -2764,17 +2690,17 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
-        <v>309</v>
+      <c r="A45" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>11</v>
@@ -2783,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="4" t="e">
@@ -2793,10 +2719,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>21</v>
@@ -2811,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="4" t="e">
@@ -2821,10 +2747,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>21</v>
@@ -2839,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="4" t="e">
@@ -2849,10 +2775,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>21</v>
@@ -2867,7 +2793,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="4" t="e">
@@ -2876,11 +2802,11 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>146</v>
+      <c r="A49" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>21</v>
@@ -2895,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="4" t="e">
@@ -2904,11 +2830,11 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
-        <v>220</v>
+      <c r="A50" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>21</v>
@@ -2923,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="4" t="e">
@@ -2932,11 +2858,11 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>147</v>
+      <c r="A51" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>21</v>
@@ -2951,7 +2877,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="4" t="e">
@@ -2961,10 +2887,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>21</v>
@@ -2979,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="4" t="e">
@@ -2988,11 +2914,11 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>124</v>
+      <c r="A53" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>21</v>
@@ -3007,7 +2933,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H53" s="13"/>
       <c r="I53" s="4" t="e">
@@ -3017,10 +2943,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>21</v>
@@ -3045,10 +2971,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>21</v>
@@ -3063,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H55" s="13"/>
       <c r="I55" s="4" t="e">
@@ -3073,10 +2999,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>21</v>
@@ -3101,10 +3027,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>21</v>
@@ -3119,7 +3045,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>26</v>
+        <v>271</v>
       </c>
       <c r="H57" s="13"/>
       <c r="I57" s="4" t="e">
@@ -3129,10 +3055,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>21</v>
@@ -3157,10 +3083,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>21</v>
@@ -3175,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="4" t="e">
@@ -3185,10 +3111,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>21</v>
@@ -3203,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H60" s="13"/>
       <c r="I60" s="4" t="e">
@@ -3213,10 +3139,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>21</v>
@@ -3231,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H61" s="13"/>
       <c r="I61" s="4" t="e">
@@ -3241,10 +3167,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>21</v>
@@ -3259,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H62" s="13"/>
       <c r="I62" s="4" t="e">
@@ -3269,10 +3195,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>21</v>
@@ -3287,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H63" s="13"/>
       <c r="I63" s="4" t="e">
@@ -3297,10 +3223,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>21</v>
@@ -3315,7 +3241,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H64" s="13"/>
       <c r="I64" s="4" t="e">
@@ -3325,10 +3251,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>21</v>
@@ -3343,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="4" t="e">
@@ -3353,10 +3279,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>21</v>
@@ -3371,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H66" s="13"/>
       <c r="I66" s="4" t="e">
@@ -3381,10 +3307,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>21</v>
@@ -3399,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H67" s="13"/>
       <c r="I67" s="4" t="e">
@@ -3409,10 +3335,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>21</v>
@@ -3427,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H68" s="13"/>
       <c r="I68" s="4" t="e">
@@ -3437,10 +3363,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>21</v>
@@ -3455,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H69" s="13"/>
       <c r="I69" s="4" t="e">
@@ -3465,10 +3391,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>21</v>
@@ -3483,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="4" t="e">
@@ -3493,10 +3419,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>21</v>
@@ -3511,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H71" s="13"/>
       <c r="I71" s="4" t="e">
@@ -3521,10 +3447,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>21</v>
@@ -3539,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H72" s="13"/>
       <c r="I72" s="4" t="e">
@@ -3549,10 +3475,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>21</v>
@@ -3567,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H73" s="13"/>
       <c r="I73" s="4" t="e">
@@ -3577,10 +3503,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>21</v>
@@ -3595,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H74" s="13"/>
       <c r="I74" s="4" t="e">
@@ -3605,10 +3531,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>21</v>
@@ -3623,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H75" s="13"/>
       <c r="I75" s="4" t="e">
@@ -3633,10 +3559,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>21</v>
@@ -3651,7 +3577,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H76" s="13"/>
       <c r="I76" s="4" t="e">
@@ -3661,10 +3587,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>21</v>
@@ -3679,7 +3605,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H77" s="13"/>
       <c r="I77" s="4" t="e">
@@ -3689,10 +3615,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>21</v>
@@ -3707,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H78" s="13"/>
       <c r="I78" s="4" t="e">
@@ -3717,10 +3643,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>21</v>
@@ -3735,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="4" t="e">
@@ -3745,10 +3671,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>21</v>
@@ -3763,7 +3689,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H80" s="13"/>
       <c r="I80" s="4" t="e">
@@ -3773,10 +3699,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>21</v>
@@ -3791,7 +3717,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H81" s="13"/>
       <c r="I81" s="4" t="e">
@@ -3801,10 +3727,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>21</v>
@@ -3819,7 +3745,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H82" s="13"/>
       <c r="I82" s="4" t="e">
@@ -3829,10 +3755,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>21</v>
@@ -3847,7 +3773,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H83" s="13"/>
       <c r="I83" s="4" t="e">
@@ -3857,10 +3783,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>21</v>
@@ -3875,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="4" t="e">
@@ -3885,10 +3811,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>21</v>
@@ -3903,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H85" s="13"/>
       <c r="I85" s="4" t="e">
@@ -3913,10 +3839,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>21</v>
@@ -3931,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H86" s="13"/>
       <c r="I86" s="4" t="e">
@@ -3941,10 +3867,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>21</v>
@@ -3959,7 +3885,7 @@
         <v>1</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="4" t="e">
@@ -3969,10 +3895,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>21</v>
@@ -3987,7 +3913,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H88" s="13"/>
       <c r="I88" s="4" t="e">
@@ -3997,10 +3923,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>21</v>
@@ -4015,7 +3941,7 @@
         <v>1</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H89" s="13"/>
       <c r="I89" s="4" t="e">
@@ -4025,10 +3951,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>21</v>
@@ -4043,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H90" s="13"/>
       <c r="I90" s="4" t="e">
@@ -4053,10 +3979,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>21</v>
@@ -4071,7 +3997,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H91" s="13"/>
       <c r="I91" s="4" t="e">
@@ -4081,10 +4007,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>21</v>
@@ -4099,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H92" s="13"/>
       <c r="I92" s="4" t="e">
@@ -4109,10 +4035,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>21</v>
@@ -4127,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H93" s="13"/>
       <c r="I93" s="4" t="e">
@@ -4137,10 +4063,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>21</v>
@@ -4165,10 +4091,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>21</v>
@@ -4183,7 +4109,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H95" s="13"/>
       <c r="I95" s="4" t="e">
@@ -4193,10 +4119,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>21</v>
@@ -4211,7 +4137,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H96" s="13"/>
       <c r="I96" s="4" t="e">
@@ -4221,10 +4147,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>21</v>
@@ -4239,7 +4165,7 @@
         <v>1</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H97" s="13"/>
       <c r="I97" s="4" t="e">
@@ -4249,10 +4175,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>21</v>
@@ -4267,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H98" s="13"/>
       <c r="I98" s="4" t="e">
@@ -4277,10 +4203,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>21</v>
@@ -4295,7 +4221,7 @@
         <v>1</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H99" s="13"/>
       <c r="I99" s="4" t="e">
@@ -4305,10 +4231,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>21</v>
@@ -4323,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H100" s="13"/>
       <c r="I100" s="4" t="e">
@@ -4342,8 +4268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EF3264-D1E6-4CF5-90F0-EEAB1E0B166B}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4624,7 +4550,7 @@
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H7&lt;&gt;"",AT指令表!H7,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H7&lt;&gt;"",AT指令表!H7,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H7&lt;&gt;"",AT指令表!H7,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H7&lt;&gt;"",AT指令表!H7,"")&amp;"\r\n""")))</f>
-        <v>"AT+WEBSOCKPORT1=6432\r\n"</v>
+        <v>"AT+MAXSK2=1\r\n"</v>
       </c>
       <c r="D7" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C7,2,LEN(C7)-IF(C7="""+++""",2,IF(C7="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4654,7 +4580,7 @@
       </c>
       <c r="K7" s="9" t="str">
         <f>IFERROR(AT指令表!I7,"")</f>
-        <v>//查询/设置WebSocket端口号</v>
+        <v>//查询/设置N号串口的最大连接数量</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -4668,7 +4594,7 @@
       </c>
       <c r="C8" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H8&lt;&gt;"",AT指令表!H8,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H8&lt;&gt;"",AT指令表!H8,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H8&lt;&gt;"",AT指令表!H8,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H8&lt;&gt;"",AT指令表!H8,"")&amp;"\r\n""")))</f>
-        <v>"AT+MAXSK2=1\r\n"</v>
+        <v>"AT+MQTTEN=ON\r\n"</v>
       </c>
       <c r="D8" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C8,2,LEN(C8)-IF(C8="""+++""",2,IF(C8="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4698,7 +4624,7 @@
       </c>
       <c r="K8" s="9" t="str">
         <f>IFERROR(AT指令表!I8,"")</f>
-        <v>//查询/设置N号串口的最大连接数量</v>
+        <v>//查询/设置MQTT网关功能状态</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4712,7 +4638,7 @@
       </c>
       <c r="C9" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H9&lt;&gt;"",AT指令表!H9,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H9&lt;&gt;"",AT指令表!H9,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H9&lt;&gt;"",AT指令表!H9,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H9&lt;&gt;"",AT指令表!H9,"")&amp;"\r\n""")))</f>
-        <v>"AT+TCPSE2=KICK\r\n"</v>
+        <v>"AT+MQTTLPORT=0\r\n"</v>
       </c>
       <c r="D9" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C9,2,LEN(C9)-IF(C9="""+++""",2,IF(C9="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4742,7 +4668,7 @@
       </c>
       <c r="K9" s="9" t="str">
         <f>IFERROR(AT指令表!I9,"")</f>
-        <v>//查询/设置N号串口的TCPS超过最大连接数的工作模式</v>
+        <v>//查询/设置MQTTsocket连接本地端口号</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -4756,7 +4682,7 @@
       </c>
       <c r="C10" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H10&lt;&gt;"",AT指令表!H10,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H10&lt;&gt;"",AT指令表!H10,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H10&lt;&gt;"",AT指令表!H10,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H10&lt;&gt;"",AT指令表!H10,"")&amp;"\r\n""")))</f>
-        <v>"AT+SOCKA2=TCPC,59.110.170.225,1883\r\n"</v>
+        <v>"AT+MQTTAUTH=ON\r\n"</v>
       </c>
       <c r="D10" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C10,2,LEN(C10)-IF(C10="""+++""",2,IF(C10="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4778,7 +4704,7 @@
       </c>
       <c r="I10" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C10,2,LEN(C10)-IF(C10="""+++""",2,IF(C10="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setRemoteIPDataLoadFun</v>
+        <v>easyATCmdDataLoadFun</v>
       </c>
       <c r="J10" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C10,2,LEN(C10)-IF(C10="""+++""",2,IF(C10="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -4786,7 +4712,7 @@
       </c>
       <c r="K10" s="9" t="str">
         <f>IFERROR(AT指令表!I10,"")</f>
-        <v>//查询/设置N号串口的socket状态（M参数为socket号）</v>
+        <v>//查询/设置MQTT连接验证开启状态</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -4800,7 +4726,7 @@
       </c>
       <c r="C11" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H11&lt;&gt;"",AT指令表!H11,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H11&lt;&gt;"",AT指令表!H11,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H11&lt;&gt;"",AT指令表!H11,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H11&lt;&gt;"",AT指令表!H11,"")&amp;"\r\n""")))</f>
-        <v>"AT+SOCKLKA2\r\n"</v>
+        <v>"AT+MQTTCID=HY_QL\r\n"</v>
       </c>
       <c r="D11" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C11,2,LEN(C11)-IF(C11="""+++""",2,IF(C11="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4830,7 +4756,7 @@
       </c>
       <c r="K11" s="9" t="str">
         <f>IFERROR(AT指令表!I11,"")</f>
-        <v>//查询N号串口的socketM的连接状态</v>
+        <v>//查询/设置MQTT客户端ID</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4844,7 +4770,7 @@
       </c>
       <c r="C12" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H12&lt;&gt;"",AT指令表!H12,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H12&lt;&gt;"",AT指令表!H12,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H12&lt;&gt;"",AT指令表!H12,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H12&lt;&gt;"",AT指令表!H12,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTEN=ON\r\n"</v>
+        <v>"AT+MQTTUSER=ql\r\n"</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C12,2,LEN(C12)-IF(C12="""+++""",2,IF(C12="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4866,7 +4792,7 @@
       </c>
       <c r="I12" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C12,2,LEN(C12)-IF(C12="""+++""",2,IF(C12="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>easyATCmdDataLoadFun</v>
+        <v>setUserAndPassWordDataLoadFun</v>
       </c>
       <c r="J12" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C12,2,LEN(C12)-IF(C12="""+++""",2,IF(C12="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -4874,7 +4800,7 @@
       </c>
       <c r="K12" s="9" t="str">
         <f>IFERROR(AT指令表!I12,"")</f>
-        <v>//查询/设置MQTT网关功能状态</v>
+        <v>//查询/设置MQTT用户名</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -4888,7 +4814,7 @@
       </c>
       <c r="C13" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H13&lt;&gt;"",AT指令表!H13,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H13&lt;&gt;"",AT指令表!H13,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H13&lt;&gt;"",AT指令表!H13,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H13&lt;&gt;"",AT指令表!H13,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTLPORT=0\r\n"</v>
+        <v>"AT+MQTTPSW=ql\r\n"</v>
       </c>
       <c r="D13" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C13,2,LEN(C13)-IF(C13="""+++""",2,IF(C13="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4910,7 +4836,7 @@
       </c>
       <c r="I13" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C13,2,LEN(C13)-IF(C13="""+++""",2,IF(C13="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>easyATCmdDataLoadFun</v>
+        <v>setUserAndPassWordDataLoadFun</v>
       </c>
       <c r="J13" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C13,2,LEN(C13)-IF(C13="""+++""",2,IF(C13="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -4918,7 +4844,7 @@
       </c>
       <c r="K13" s="9" t="str">
         <f>IFERROR(AT指令表!I13,"")</f>
-        <v>//查询/设置MQTTsocket连接本地端口号</v>
+        <v>//查询/设置MQTT用户密码</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -4932,7 +4858,7 @@
       </c>
       <c r="C14" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H14&lt;&gt;"",AT指令表!H14,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H14&lt;&gt;"",AT指令表!H14,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H14&lt;&gt;"",AT指令表!H14,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H14&lt;&gt;"",AT指令表!H14,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTAUTH=ON\r\n"</v>
+        <v>"AT+MQTTPUBCUSEN=OFF\r\n"</v>
       </c>
       <c r="D14" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C14,2,LEN(C14)-IF(C14="""+++""",2,IF(C14="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4962,7 +4888,7 @@
       </c>
       <c r="K14" s="9" t="str">
         <f>IFERROR(AT指令表!I14,"")</f>
-        <v>//查询/设置MQTT连接验证开启状态</v>
+        <v>//查询/设置MQTT主题发布自定义模式</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -4976,7 +4902,7 @@
       </c>
       <c r="C15" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H15&lt;&gt;"",AT指令表!H15,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H15&lt;&gt;"",AT指令表!H15,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H15&lt;&gt;"",AT指令表!H15,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H15&lt;&gt;"",AT指令表!H15,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTCID=HY_QL\r\n"</v>
+        <v>"AT+MQTTPUB=1,ON,hy/gw/set/02345678903,0,MY_PUB,0,OFF,3\r\n"</v>
       </c>
       <c r="D15" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C15,2,LEN(C15)-IF(C15="""+++""",2,IF(C15="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -4998,7 +4924,7 @@
       </c>
       <c r="I15" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C15,2,LEN(C15)-IF(C15="""+++""",2,IF(C15="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>easyATCmdDataLoadFun</v>
+        <v>setMQTTMassagePUBFun</v>
       </c>
       <c r="J15" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C15,2,LEN(C15)-IF(C15="""+++""",2,IF(C15="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5006,7 +4932,7 @@
       </c>
       <c r="K15" s="9" t="str">
         <f>IFERROR(AT指令表!I15,"")</f>
-        <v>//查询/设置MQTT客户端ID</v>
+        <v>//查询/设置MQTT的预置发布主题信息</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -5020,7 +4946,7 @@
       </c>
       <c r="C16" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H16&lt;&gt;"",AT指令表!H16,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H16&lt;&gt;"",AT指令表!H16,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H16&lt;&gt;"",AT指令表!H16,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H16&lt;&gt;"",AT指令表!H16,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTUSER=ql\r\n"</v>
+        <v>"AT+MQTTSUB=1,ON,hy/gw/get/02345678903,0,0,&amp;#44,3\r\n"</v>
       </c>
       <c r="D16" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C16,2,LEN(C16)-IF(C16="""+++""",2,IF(C16="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -5042,7 +4968,7 @@
       </c>
       <c r="I16" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C16,2,LEN(C16)-IF(C16="""+++""",2,IF(C16="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setUserAndPassWordDataLoadFun</v>
+        <v>setMQTTMassageSUBFun</v>
       </c>
       <c r="J16" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C16,2,LEN(C16)-IF(C16="""+++""",2,IF(C16="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5050,7 +4976,7 @@
       </c>
       <c r="K16" s="9" t="str">
         <f>IFERROR(AT指令表!I16,"")</f>
-        <v>//查询/设置MQTT用户名</v>
+        <v>//查询/设置MQTT的预置订阅主题信息</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -5064,7 +4990,7 @@
       </c>
       <c r="C17" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H17&lt;&gt;"",AT指令表!H17,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H17&lt;&gt;"",AT指令表!H17,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H17&lt;&gt;"",AT指令表!H17,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H17&lt;&gt;"",AT指令表!H17,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTPSW=ql\r\n"</v>
+        <v>"AT+MQTTSER=59.110.170.225,1883\r\n"</v>
       </c>
       <c r="D17" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C17,2,LEN(C17)-IF(C17="""+++""",2,IF(C17="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -5086,7 +5012,7 @@
       </c>
       <c r="I17" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C17,2,LEN(C17)-IF(C17="""+++""",2,IF(C17="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setUserAndPassWordDataLoadFun</v>
+        <v>setRemoteIPDataLoadFun</v>
       </c>
       <c r="J17" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C17,2,LEN(C17)-IF(C17="""+++""",2,IF(C17="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5094,7 +5020,7 @@
       </c>
       <c r="K17" s="9" t="str">
         <f>IFERROR(AT指令表!I17,"")</f>
-        <v>//查询/设置MQTT用户密码</v>
+        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -5104,11 +5030,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H18&lt;&gt;"",AT指令表!H18,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H18&lt;&gt;"",AT指令表!H18,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H18&lt;&gt;"",AT指令表!H18,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H18&lt;&gt;"",AT指令表!H18,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTPUBCUSEN=ON\r\n"</v>
+        <v>"AT+Z\r\n"</v>
       </c>
       <c r="D18" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C18,2,LEN(C18)-IF(C18="""+++""",2,IF(C18="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
@@ -5138,7 +5064,7 @@
       </c>
       <c r="K18" s="9" t="str">
         <f>IFERROR(AT指令表!I18,"")</f>
-        <v>//查询/设置MQTT主题发布自定义模式</v>
+        <v>//设备重启</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -5148,19 +5074,19 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>-1</v>
       </c>
       <c r="C19" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H19&lt;&gt;"",AT指令表!H19,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H19&lt;&gt;"",AT指令表!H19,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H19&lt;&gt;"",AT指令表!H19,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H19&lt;&gt;"",AT指令表!H19,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTPUB=1,ON,hy/gw/get/02345678903,0,MY_PUB,0,OFF,2\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D19" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C19,2,LEN(C19)-IF(C19="""+++""",2,IF(C19="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C19,2,LEN(C19)-IF(C19="""+++""",2,IF(C19="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
@@ -5170,11 +5096,11 @@
       </c>
       <c r="H19" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C19,2,LEN(C19)-IF(C19="""+++""",2,IF(C19="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I19" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C19,2,LEN(C19)-IF(C19="""+++""",2,IF(C19="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setMQTTMassagePUBFun</v>
+        <v>easyATCmdDataLoadFun</v>
       </c>
       <c r="J19" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C19,2,LEN(C19)-IF(C19="""+++""",2,IF(C19="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5182,7 +5108,7 @@
       </c>
       <c r="K19" s="9" t="str">
         <f>IFERROR(AT指令表!I19,"")</f>
-        <v>//查询/设置MQTT的预置发布主题信息</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -5192,19 +5118,19 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H20&lt;&gt;"",AT指令表!H20,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H20&lt;&gt;"",AT指令表!H20,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H20&lt;&gt;"",AT指令表!H20,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H20&lt;&gt;"",AT指令表!H20,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTSUB=1,ON,/hy/gw/#,0,0,&amp;#44,2\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D20" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C20,2,LEN(C20)-IF(C20="""+++""",2,IF(C20="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C20,2,LEN(C20)-IF(C20="""+++""",2,IF(C20="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
@@ -5214,11 +5140,11 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C20,2,LEN(C20)-IF(C20="""+++""",2,IF(C20="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I20" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C20,2,LEN(C20)-IF(C20="""+++""",2,IF(C20="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setMQTTMassageSUBFun</v>
+        <v>easyATCmdDataLoadFun</v>
       </c>
       <c r="J20" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C20,2,LEN(C20)-IF(C20="""+++""",2,IF(C20="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5226,7 +5152,7 @@
       </c>
       <c r="K20" s="9" t="str">
         <f>IFERROR(AT指令表!I20,"")</f>
-        <v>//查询/设置MQTT的预置订阅主题信息</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -5236,19 +5162,19 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H21&lt;&gt;"",AT指令表!H21,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H21&lt;&gt;"",AT指令表!H21,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H21&lt;&gt;"",AT指令表!H21,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H21&lt;&gt;"",AT指令表!H21,"")&amp;"\r\n""")))</f>
-        <v>"AT+MQTTSER=59.110.170.225,1883\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D21" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C21,2,LEN(C21)-IF(C21="""+++""",2,IF(C21="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C21,2,LEN(C21)-IF(C21="""+++""",2,IF(C21="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F21" s="1">
         <v>3</v>
@@ -5258,11 +5184,11 @@
       </c>
       <c r="H21" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C21,2,LEN(C21)-IF(C21="""+++""",2,IF(C21="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C21,2,LEN(C21)-IF(C21="""+++""",2,IF(C21="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
-        <v>setRemoteIPDataLoadFun</v>
+        <v>easyATCmdDataLoadFun</v>
       </c>
       <c r="J21" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C21,2,LEN(C21)-IF(C21="""+++""",2,IF(C21="""a""",2,6))),AT指令表!A:F,5,0),"easyATCmdDataDoingFun")</f>
@@ -5270,7 +5196,7 @@
       </c>
       <c r="K21" s="9" t="str">
         <f>IFERROR(AT指令表!I21,"")</f>
-        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -5280,19 +5206,19 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>-1</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H22&lt;&gt;"",AT指令表!H22,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H22&lt;&gt;"",AT指令表!H22,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H22&lt;&gt;"",AT指令表!H22,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H22&lt;&gt;"",AT指令表!H22,"")&amp;"\r\n""")))</f>
-        <v>"AT+MID=NJHY\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D22" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C22,2,LEN(C22)-IF(C22="""+++""",2,IF(C22="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C22,2,LEN(C22)-IF(C22="""+++""",2,IF(C22="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F22" s="1">
         <v>3</v>
@@ -5302,7 +5228,7 @@
       </c>
       <c r="H22" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C22,2,LEN(C22)-IF(C22="""+++""",2,IF(C22="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I22" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C22,2,LEN(C22)-IF(C22="""+++""",2,IF(C22="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
@@ -5314,7 +5240,7 @@
       </c>
       <c r="K22" s="9" t="str">
         <f>IFERROR(AT指令表!I22,"")</f>
-        <v>//查询/设置模块名称</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -5324,19 +5250,19 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>-1</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H23&lt;&gt;"",AT指令表!H23,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H23&lt;&gt;"",AT指令表!H23,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H23&lt;&gt;"",AT指令表!H23,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H23&lt;&gt;"",AT指令表!H23,"")&amp;"\r\n""")))</f>
-        <v>"AT+WEBPOINT=OFF\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D23" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C23,2,LEN(C23)-IF(C23="""+++""",2,IF(C23="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C23,2,LEN(C23)-IF(C23="""+++""",2,IF(C23="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F23" s="1">
         <v>3</v>
@@ -5346,7 +5272,7 @@
       </c>
       <c r="H23" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C23,2,LEN(C23)-IF(C23="""+++""",2,IF(C23="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I23" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C23,2,LEN(C23)-IF(C23="""+++""",2,IF(C23="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
@@ -5358,7 +5284,7 @@
       </c>
       <c r="K23" s="9" t="str">
         <f>IFERROR(AT指令表!I23,"")</f>
-        <v>//查询/设置WebSocket的方向</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -5368,19 +5294,19 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>-1</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H24&lt;&gt;"",AT指令表!H24,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H24&lt;&gt;"",AT指令表!H24,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H24&lt;&gt;"",AT指令表!H24,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H24&lt;&gt;"",AT指令表!H24,"")&amp;"\r\n""")))</f>
-        <v>"AT+CFGTF\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D24" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C24,2,LEN(C24)-IF(C24="""+++""",2,IF(C24="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C24,2,LEN(C24)-IF(C24="""+++""",2,IF(C24="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F24" s="1">
         <v>3</v>
@@ -5390,7 +5316,7 @@
       </c>
       <c r="H24" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C24,2,LEN(C24)-IF(C24="""+++""",2,IF(C24="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I24" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C24,2,LEN(C24)-IF(C24="""+++""",2,IF(C24="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
@@ -5402,7 +5328,7 @@
       </c>
       <c r="K24" s="9" t="str">
         <f>IFERROR(AT指令表!I24,"")</f>
-        <v>//设置将当前参数保存为用户默认参数</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -5416,15 +5342,15 @@
       </c>
       <c r="C25" s="4" t="str">
         <f>IF(""""&amp;IF(AT指令表!H25&lt;&gt;"",AT指令表!H25,"")&amp;""""="""+++""","""+++""",IF(""""&amp;IF(AT指令表!H25&lt;&gt;"",AT指令表!H25,"")&amp;""""="""a""","""a""",IF(""""&amp;IF(AT指令表!H25&lt;&gt;"",AT指令表!H25,"")&amp;""""="""""","""""",""""&amp;IF(AT指令表!H25&lt;&gt;"",AT指令表!H25,"")&amp;"\r\n""")))</f>
-        <v>"AT+Z\r\n"</v>
+        <v>""</v>
       </c>
       <c r="D25" s="4" t="str">
         <f>IFERROR(VLOOKUP(MID(C25,2,LEN(C25)-IF(C25="""+++""",2,IF(C25="""a""",2,6))),AT指令表!A:B,2,0),"""""")</f>
-        <v>"+OK"</v>
+        <v>""</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C25,2,LEN(C25)-IF(C25="""+++""",2,IF(C25="""a""",2,6))),AT指令表!A:F,6,0)=1,"true","false"),"error")</f>
-        <v>true</v>
+        <v>error</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -5434,7 +5360,7 @@
       </c>
       <c r="H25" s="1" t="str">
         <f>IFERROR(IF(VLOOKUP(MID(C25,2,LEN(C25)-IF(C25="""+++""",2,IF(C25="""a""",2,6))),AT指令表!A:C,3,0)=1,"true","false"),"error")</f>
-        <v>false</v>
+        <v>error</v>
       </c>
       <c r="I25" s="1" t="str">
         <f>IFERROR(VLOOKUP(MID(C25,2,LEN(C25)-IF(C25="""+++""",2,IF(C25="""a""",2,6))),AT指令表!A:F,4,0),"easyATCmdDataLoadFun")</f>
@@ -5446,7 +5372,7 @@
       </c>
       <c r="K25" s="9" t="str">
         <f>IFERROR(AT指令表!I25,"")</f>
-        <v>//设备重启</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -6340,8 +6266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60290CD1-5C1F-452D-8581-756D4E80FE33}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B45" sqref="A2:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6409,191 +6335,191 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A7&amp;","&amp;AT指令代码格式!B7&amp;","&amp;AT指令代码格式!C7&amp;","&amp;AT指令代码格式!D7&amp;","&amp;IF(AT指令代码格式!E7="error","false",AT指令代码格式!E7)&amp;","&amp;AT指令代码格式!F7&amp;","&amp;AT指令代码格式!G7&amp;","&amp;IF(AT指令代码格式!H7="error","false",AT指令代码格式!H7)&amp;","&amp;AT指令代码格式!I7&amp;","&amp;AT指令代码格式!J7&amp;", NULL, NULL},"</f>
-        <v>{5,6,"AT+WEBSOCKPORT1=6432\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{5,6,"AT+MAXSK2=1\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B7" s="11" t="str">
         <f>AT指令代码格式!K7</f>
-        <v>//查询/设置WebSocket端口号</v>
+        <v>//查询/设置N号串口的最大连接数量</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A8&amp;","&amp;AT指令代码格式!B8&amp;","&amp;AT指令代码格式!C8&amp;","&amp;AT指令代码格式!D8&amp;","&amp;IF(AT指令代码格式!E8="error","false",AT指令代码格式!E8)&amp;","&amp;AT指令代码格式!F8&amp;","&amp;AT指令代码格式!G8&amp;","&amp;IF(AT指令代码格式!H8="error","false",AT指令代码格式!H8)&amp;","&amp;AT指令代码格式!I8&amp;","&amp;AT指令代码格式!J8&amp;", NULL, NULL},"</f>
-        <v>{6,7,"AT+MAXSK2=1\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{6,7,"AT+MQTTEN=ON\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B8" s="11" t="str">
         <f>AT指令代码格式!K8</f>
-        <v>//查询/设置N号串口的最大连接数量</v>
+        <v>//查询/设置MQTT网关功能状态</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A9&amp;","&amp;AT指令代码格式!B9&amp;","&amp;AT指令代码格式!C9&amp;","&amp;AT指令代码格式!D9&amp;","&amp;IF(AT指令代码格式!E9="error","false",AT指令代码格式!E9)&amp;","&amp;AT指令代码格式!F9&amp;","&amp;AT指令代码格式!G9&amp;","&amp;IF(AT指令代码格式!H9="error","false",AT指令代码格式!H9)&amp;","&amp;AT指令代码格式!I9&amp;","&amp;AT指令代码格式!J9&amp;", NULL, NULL},"</f>
-        <v>{7,8,"AT+TCPSE2=KICK\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{7,8,"AT+MQTTLPORT=0\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B9" s="11" t="str">
         <f>AT指令代码格式!K9</f>
-        <v>//查询/设置N号串口的TCPS超过最大连接数的工作模式</v>
+        <v>//查询/设置MQTTsocket连接本地端口号</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A10&amp;","&amp;AT指令代码格式!B10&amp;","&amp;AT指令代码格式!C10&amp;","&amp;AT指令代码格式!D10&amp;","&amp;IF(AT指令代码格式!E10="error","false",AT指令代码格式!E10)&amp;","&amp;AT指令代码格式!F10&amp;","&amp;AT指令代码格式!G10&amp;","&amp;IF(AT指令代码格式!H10="error","false",AT指令代码格式!H10)&amp;","&amp;AT指令代码格式!I10&amp;","&amp;AT指令代码格式!J10&amp;", NULL, NULL},"</f>
-        <v>{8,9,"AT+SOCKA2=TCPC,59.110.170.225,1883\r\n","+OK",true,3,3,false,setRemoteIPDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{8,9,"AT+MQTTAUTH=ON\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B10" s="11" t="str">
         <f>AT指令代码格式!K10</f>
-        <v>//查询/设置N号串口的socket状态（M参数为socket号）</v>
+        <v>//查询/设置MQTT连接验证开启状态</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A11&amp;","&amp;AT指令代码格式!B11&amp;","&amp;AT指令代码格式!C11&amp;","&amp;AT指令代码格式!D11&amp;","&amp;IF(AT指令代码格式!E11="error","false",AT指令代码格式!E11)&amp;","&amp;AT指令代码格式!F11&amp;","&amp;AT指令代码格式!G11&amp;","&amp;IF(AT指令代码格式!H11="error","false",AT指令代码格式!H11)&amp;","&amp;AT指令代码格式!I11&amp;","&amp;AT指令代码格式!J11&amp;", NULL, NULL},"</f>
-        <v>{9,10,"AT+SOCKLKA2\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{9,10,"AT+MQTTCID=HY_QL\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B11" s="11" t="str">
         <f>AT指令代码格式!K11</f>
-        <v>//查询N号串口的socketM的连接状态</v>
+        <v>//查询/设置MQTT客户端ID</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A12&amp;","&amp;AT指令代码格式!B12&amp;","&amp;AT指令代码格式!C12&amp;","&amp;AT指令代码格式!D12&amp;","&amp;IF(AT指令代码格式!E12="error","false",AT指令代码格式!E12)&amp;","&amp;AT指令代码格式!F12&amp;","&amp;AT指令代码格式!G12&amp;","&amp;IF(AT指令代码格式!H12="error","false",AT指令代码格式!H12)&amp;","&amp;AT指令代码格式!I12&amp;","&amp;AT指令代码格式!J12&amp;", NULL, NULL},"</f>
-        <v>{10,11,"AT+MQTTEN=ON\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{10,11,"AT+MQTTUSER=ql\r\n","+OK",true,3,3,false,setUserAndPassWordDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B12" s="11" t="str">
         <f>AT指令代码格式!K12</f>
-        <v>//查询/设置MQTT网关功能状态</v>
+        <v>//查询/设置MQTT用户名</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A13&amp;","&amp;AT指令代码格式!B13&amp;","&amp;AT指令代码格式!C13&amp;","&amp;AT指令代码格式!D13&amp;","&amp;IF(AT指令代码格式!E13="error","false",AT指令代码格式!E13)&amp;","&amp;AT指令代码格式!F13&amp;","&amp;AT指令代码格式!G13&amp;","&amp;IF(AT指令代码格式!H13="error","false",AT指令代码格式!H13)&amp;","&amp;AT指令代码格式!I13&amp;","&amp;AT指令代码格式!J13&amp;", NULL, NULL},"</f>
-        <v>{11,12,"AT+MQTTLPORT=0\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{11,12,"AT+MQTTPSW=ql\r\n","+OK",true,3,3,false,setUserAndPassWordDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B13" s="11" t="str">
         <f>AT指令代码格式!K13</f>
-        <v>//查询/设置MQTTsocket连接本地端口号</v>
+        <v>//查询/设置MQTT用户密码</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A14&amp;","&amp;AT指令代码格式!B14&amp;","&amp;AT指令代码格式!C14&amp;","&amp;AT指令代码格式!D14&amp;","&amp;IF(AT指令代码格式!E14="error","false",AT指令代码格式!E14)&amp;","&amp;AT指令代码格式!F14&amp;","&amp;AT指令代码格式!G14&amp;","&amp;IF(AT指令代码格式!H14="error","false",AT指令代码格式!H14)&amp;","&amp;AT指令代码格式!I14&amp;","&amp;AT指令代码格式!J14&amp;", NULL, NULL},"</f>
-        <v>{12,13,"AT+MQTTAUTH=ON\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{12,13,"AT+MQTTPUBCUSEN=OFF\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B14" s="11" t="str">
         <f>AT指令代码格式!K14</f>
-        <v>//查询/设置MQTT连接验证开启状态</v>
+        <v>//查询/设置MQTT主题发布自定义模式</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A15&amp;","&amp;AT指令代码格式!B15&amp;","&amp;AT指令代码格式!C15&amp;","&amp;AT指令代码格式!D15&amp;","&amp;IF(AT指令代码格式!E15="error","false",AT指令代码格式!E15)&amp;","&amp;AT指令代码格式!F15&amp;","&amp;AT指令代码格式!G15&amp;","&amp;IF(AT指令代码格式!H15="error","false",AT指令代码格式!H15)&amp;","&amp;AT指令代码格式!I15&amp;","&amp;AT指令代码格式!J15&amp;", NULL, NULL},"</f>
-        <v>{13,14,"AT+MQTTCID=HY_QL\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{13,14,"AT+MQTTPUB=1,ON,hy/gw/set/02345678903,0,MY_PUB,0,OFF,3\r\n","+OK",true,3,3,false,setMQTTMassagePUBFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B15" s="11" t="str">
         <f>AT指令代码格式!K15</f>
-        <v>//查询/设置MQTT客户端ID</v>
+        <v>//查询/设置MQTT的预置发布主题信息</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A16&amp;","&amp;AT指令代码格式!B16&amp;","&amp;AT指令代码格式!C16&amp;","&amp;AT指令代码格式!D16&amp;","&amp;IF(AT指令代码格式!E16="error","false",AT指令代码格式!E16)&amp;","&amp;AT指令代码格式!F16&amp;","&amp;AT指令代码格式!G16&amp;","&amp;IF(AT指令代码格式!H16="error","false",AT指令代码格式!H16)&amp;","&amp;AT指令代码格式!I16&amp;","&amp;AT指令代码格式!J16&amp;", NULL, NULL},"</f>
-        <v>{14,15,"AT+MQTTUSER=ql\r\n","+OK",true,3,3,false,setUserAndPassWordDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{14,15,"AT+MQTTSUB=1,ON,hy/gw/get/02345678903,0,0,&amp;#44,3\r\n","+OK",true,3,3,false,setMQTTMassageSUBFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B16" s="11" t="str">
         <f>AT指令代码格式!K16</f>
-        <v>//查询/设置MQTT用户名</v>
+        <v>//查询/设置MQTT的预置订阅主题信息</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A17&amp;","&amp;AT指令代码格式!B17&amp;","&amp;AT指令代码格式!C17&amp;","&amp;AT指令代码格式!D17&amp;","&amp;IF(AT指令代码格式!E17="error","false",AT指令代码格式!E17)&amp;","&amp;AT指令代码格式!F17&amp;","&amp;AT指令代码格式!G17&amp;","&amp;IF(AT指令代码格式!H17="error","false",AT指令代码格式!H17)&amp;","&amp;AT指令代码格式!I17&amp;","&amp;AT指令代码格式!J17&amp;", NULL, NULL},"</f>
-        <v>{15,16,"AT+MQTTPSW=ql\r\n","+OK",true,3,3,false,setUserAndPassWordDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{15,16,"AT+MQTTSER=59.110.170.225,1883\r\n","+OK",true,3,3,false,setRemoteIPDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B17" s="11" t="str">
         <f>AT指令代码格式!K17</f>
-        <v>//查询/设置MQTT用户密码</v>
+        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A18&amp;","&amp;AT指令代码格式!B18&amp;","&amp;AT指令代码格式!C18&amp;","&amp;AT指令代码格式!D18&amp;","&amp;IF(AT指令代码格式!E18="error","false",AT指令代码格式!E18)&amp;","&amp;AT指令代码格式!F18&amp;","&amp;AT指令代码格式!G18&amp;","&amp;IF(AT指令代码格式!H18="error","false",AT指令代码格式!H18)&amp;","&amp;AT指令代码格式!I18&amp;","&amp;AT指令代码格式!J18&amp;", NULL, NULL},"</f>
-        <v>{16,17,"AT+MQTTPUBCUSEN=ON\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{16,-1,"AT+Z\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B18" s="11" t="str">
         <f>AT指令代码格式!K18</f>
-        <v>//查询/设置MQTT主题发布自定义模式</v>
+        <v>//设备重启</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A19&amp;","&amp;AT指令代码格式!B19&amp;","&amp;AT指令代码格式!C19&amp;","&amp;AT指令代码格式!D19&amp;","&amp;IF(AT指令代码格式!E19="error","false",AT指令代码格式!E19)&amp;","&amp;AT指令代码格式!F19&amp;","&amp;AT指令代码格式!G19&amp;","&amp;IF(AT指令代码格式!H19="error","false",AT指令代码格式!H19)&amp;","&amp;AT指令代码格式!I19&amp;","&amp;AT指令代码格式!J19&amp;", NULL, NULL},"</f>
-        <v>{17,18,"AT+MQTTPUB=1,ON,hy/gw/get/02345678903,0,MY_PUB,0,OFF,2\r\n","+OK",true,3,3,false,setMQTTMassagePUBFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{17,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B19" s="11" t="str">
         <f>AT指令代码格式!K19</f>
-        <v>//查询/设置MQTT的预置发布主题信息</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A20&amp;","&amp;AT指令代码格式!B20&amp;","&amp;AT指令代码格式!C20&amp;","&amp;AT指令代码格式!D20&amp;","&amp;IF(AT指令代码格式!E20="error","false",AT指令代码格式!E20)&amp;","&amp;AT指令代码格式!F20&amp;","&amp;AT指令代码格式!G20&amp;","&amp;IF(AT指令代码格式!H20="error","false",AT指令代码格式!H20)&amp;","&amp;AT指令代码格式!I20&amp;","&amp;AT指令代码格式!J20&amp;", NULL, NULL},"</f>
-        <v>{18,19,"AT+MQTTSUB=1,ON,/hy/gw/#,0,0,&amp;#44,2\r\n","+OK",true,3,3,false,setMQTTMassageSUBFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{18,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B20" s="11" t="str">
         <f>AT指令代码格式!K20</f>
-        <v>//查询/设置MQTT的预置订阅主题信息</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A21&amp;","&amp;AT指令代码格式!B21&amp;","&amp;AT指令代码格式!C21&amp;","&amp;AT指令代码格式!D21&amp;","&amp;IF(AT指令代码格式!E21="error","false",AT指令代码格式!E21)&amp;","&amp;AT指令代码格式!F21&amp;","&amp;AT指令代码格式!G21&amp;","&amp;IF(AT指令代码格式!H21="error","false",AT指令代码格式!H21)&amp;","&amp;AT指令代码格式!I21&amp;","&amp;AT指令代码格式!J21&amp;", NULL, NULL},"</f>
-        <v>{19,20,"AT+MQTTSER=59.110.170.225,1883\r\n","+OK",true,3,3,false,setRemoteIPDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{19,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B21" s="11" t="str">
         <f>AT指令代码格式!K21</f>
-        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A22&amp;","&amp;AT指令代码格式!B22&amp;","&amp;AT指令代码格式!C22&amp;","&amp;AT指令代码格式!D22&amp;","&amp;IF(AT指令代码格式!E22="error","false",AT指令代码格式!E22)&amp;","&amp;AT指令代码格式!F22&amp;","&amp;AT指令代码格式!G22&amp;","&amp;IF(AT指令代码格式!H22="error","false",AT指令代码格式!H22)&amp;","&amp;AT指令代码格式!I22&amp;","&amp;AT指令代码格式!J22&amp;", NULL, NULL},"</f>
-        <v>{20,21,"AT+MID=NJHY\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{20,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B22" s="11" t="str">
         <f>AT指令代码格式!K22</f>
-        <v>//查询/设置模块名称</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A23&amp;","&amp;AT指令代码格式!B23&amp;","&amp;AT指令代码格式!C23&amp;","&amp;AT指令代码格式!D23&amp;","&amp;IF(AT指令代码格式!E23="error","false",AT指令代码格式!E23)&amp;","&amp;AT指令代码格式!F23&amp;","&amp;AT指令代码格式!G23&amp;","&amp;IF(AT指令代码格式!H23="error","false",AT指令代码格式!H23)&amp;","&amp;AT指令代码格式!I23&amp;","&amp;AT指令代码格式!J23&amp;", NULL, NULL},"</f>
-        <v>{21,22,"AT+WEBPOINT=OFF\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{21,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B23" s="11" t="str">
         <f>AT指令代码格式!K23</f>
-        <v>//查询/设置WebSocket的方向</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A24&amp;","&amp;AT指令代码格式!B24&amp;","&amp;AT指令代码格式!C24&amp;","&amp;AT指令代码格式!D24&amp;","&amp;IF(AT指令代码格式!E24="error","false",AT指令代码格式!E24)&amp;","&amp;AT指令代码格式!F24&amp;","&amp;AT指令代码格式!G24&amp;","&amp;IF(AT指令代码格式!H24="error","false",AT指令代码格式!H24)&amp;","&amp;AT指令代码格式!I24&amp;","&amp;AT指令代码格式!J24&amp;", NULL, NULL},"</f>
-        <v>{22,23,"AT+CFGTF\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{22,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B24" s="11" t="str">
         <f>AT指令代码格式!K24</f>
-        <v>//设置将当前参数保存为用户默认参数</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="str">
         <f>"{"&amp;AT指令代码格式!A25&amp;","&amp;AT指令代码格式!B25&amp;","&amp;AT指令代码格式!C25&amp;","&amp;AT指令代码格式!D25&amp;","&amp;IF(AT指令代码格式!E25="error","false",AT指令代码格式!E25)&amp;","&amp;AT指令代码格式!F25&amp;","&amp;AT指令代码格式!G25&amp;","&amp;IF(AT指令代码格式!H25="error","false",AT指令代码格式!H25)&amp;","&amp;AT指令代码格式!I25&amp;","&amp;AT指令代码格式!J25&amp;", NULL, NULL},"</f>
-        <v>{23,-1,"AT+Z\r\n","+OK",true,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
+        <v>{23,-1,"","",false,3,3,false,easyATCmdDataLoadFun,easyATCmdDataDoingFun, NULL, NULL},</v>
       </c>
       <c r="B25" s="11" t="str">
         <f>AT指令代码格式!K25</f>
-        <v>//设备重启</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -6805,410 +6731,462 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26FA53E-F5FF-4E5E-B2D8-E9E696CBA27B}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.25" customWidth="1"/>
-    <col min="2" max="2" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f>AT指令表!H2</f>
+        <v>AT+E=ON</v>
+      </c>
+      <c r="F5" t="str">
+        <f>AT指令表!I2</f>
+        <v>//查询/设置回显使能</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f>AT指令表!H3</f>
+        <v>AT+UART2=115200,8,1,NONE,NFC</v>
+      </c>
+      <c r="F6" t="str">
+        <f>AT指令表!I3</f>
+        <v>//查询/设置N号串口接口参数</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f>AT指令表!H4</f>
+        <v>AT+UARTCLBUF=ON</v>
+      </c>
+      <c r="F7" t="str">
+        <f>AT指令表!I4</f>
+        <v>//查询/设置连接前是否清理串口缓存</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f>AT指令表!H5</f>
+        <v>AT+DNSTYPE=AUTO</v>
+      </c>
+      <c r="F8" t="str">
+        <f>AT指令表!I5</f>
+        <v>//查询/设置模块DNS获取方式</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>AT指令表!H6</f>
+        <v>AT+WANN=STATIC,192.168.1.117,255.255.255.0,192.168.1.1</v>
+      </c>
+      <c r="F9" t="str">
+        <f>AT指令表!I6</f>
+        <v>//查询/设置模块获取到的WAN口IP（DHCP/STATIC）</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f>AT指令表!H7</f>
+        <v>AT+MAXSK2=1</v>
+      </c>
+      <c r="F10" t="str">
+        <f>AT指令表!I7</f>
+        <v>//查询/设置N号串口的最大连接数量</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f>AT指令表!H8</f>
+        <v>AT+MQTTEN=ON</v>
+      </c>
+      <c r="F11" t="str">
+        <f>AT指令表!I8</f>
+        <v>//查询/设置MQTT网关功能状态</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="6" t="str">
+        <f>AT指令表!H9</f>
+        <v>AT+MQTTLPORT=0</v>
+      </c>
+      <c r="F12" t="str">
+        <f>AT指令表!I9</f>
+        <v>//查询/设置MQTTsocket连接本地端口号</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E13" s="6" t="str">
+        <f>AT指令表!H10</f>
+        <v>AT+MQTTAUTH=ON</v>
+      </c>
+      <c r="F13" t="str">
+        <f>AT指令表!I10</f>
+        <v>//查询/设置MQTT连接验证开启状态</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E14" s="6" t="str">
+        <f>AT指令表!H11</f>
+        <v>AT+MQTTCID=HY_QL</v>
+      </c>
+      <c r="F14" t="str">
+        <f>AT指令表!I11</f>
+        <v>//查询/设置MQTT客户端ID</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f>AT指令表!H12</f>
+        <v>AT+MQTTUSER=ql</v>
+      </c>
+      <c r="F15" t="str">
+        <f>AT指令表!I12</f>
+        <v>//查询/设置MQTT用户名</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f>AT指令表!H13</f>
+        <v>AT+MQTTPSW=ql</v>
+      </c>
+      <c r="F16" t="str">
+        <f>AT指令表!I13</f>
+        <v>//查询/设置MQTT用户密码</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f>AT指令表!H14</f>
+        <v>AT+MQTTPUBCUSEN=OFF</v>
+      </c>
+      <c r="F17" t="str">
+        <f>AT指令表!I14</f>
+        <v>//查询/设置MQTT主题发布自定义模式</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D18" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E18" s="6" t="str">
+        <f>AT指令表!H15</f>
+        <v>AT+MQTTPUB=1,ON,hy/gw/set/02345678903,0,MY_PUB,0,OFF,3</v>
+      </c>
+      <c r="F18" t="str">
+        <f>AT指令表!I15</f>
+        <v>//查询/设置MQTT的预置发布主题信息</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D19" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="D2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E19" s="6" t="str">
+        <f>AT指令表!H16</f>
+        <v>AT+MQTTSUB=1,ON,hy/gw/get/02345678903,0,0,&amp;#44,3</v>
+      </c>
+      <c r="F19" t="str">
+        <f>AT指令表!I16</f>
+        <v>//查询/设置MQTT的预置订阅主题信息</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D20" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E20" s="6" t="str">
+        <f>AT指令表!H17</f>
+        <v>AT+MQTTSER=59.110.170.225,1883</v>
+      </c>
+      <c r="F20" t="str">
+        <f>AT指令表!I17</f>
+        <v>//查询/设置MQTT网关功能的服务器IP地址，端口号</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D21" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" t="s">
-        <v>257</v>
-      </c>
-      <c r="D5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>212</v>
-      </c>
-      <c r="B6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C10" t="s">
-        <v>267</v>
-      </c>
-      <c r="D10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B12" t="s">
-        <v>270</v>
-      </c>
-      <c r="C12" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C13" t="s">
-        <v>273</v>
-      </c>
-      <c r="D13" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>227</v>
-      </c>
-      <c r="B14" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" t="s">
-        <v>275</v>
-      </c>
-      <c r="D14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B15" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" t="s">
-        <v>277</v>
-      </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>229</v>
-      </c>
-      <c r="B16" t="s">
-        <v>278</v>
-      </c>
-      <c r="C16" t="s">
-        <v>279</v>
-      </c>
-      <c r="D16" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B17" t="s">
-        <v>280</v>
-      </c>
-      <c r="C17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>232</v>
-      </c>
-      <c r="B18" t="s">
-        <v>282</v>
-      </c>
-      <c r="C18" t="s">
-        <v>283</v>
-      </c>
-      <c r="D18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>234</v>
-      </c>
-      <c r="B19" t="s">
-        <v>284</v>
-      </c>
-      <c r="C19" t="s">
-        <v>285</v>
-      </c>
-      <c r="D19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B20" t="s">
-        <v>286</v>
-      </c>
-      <c r="C20" t="s">
-        <v>287</v>
-      </c>
-      <c r="D20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22" t="s">
-        <v>290</v>
-      </c>
-      <c r="C22" t="s">
-        <v>291</v>
-      </c>
-      <c r="D22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>241</v>
-      </c>
-      <c r="B23" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" t="s">
-        <v>293</v>
-      </c>
-      <c r="D23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>243</v>
-      </c>
-      <c r="B24" t="s">
-        <v>294</v>
-      </c>
-      <c r="C24" t="s">
-        <v>295</v>
-      </c>
-      <c r="D24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B25" t="s">
-        <v>296</v>
-      </c>
-      <c r="C25" t="s">
-        <v>297</v>
-      </c>
-      <c r="D25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>245</v>
-      </c>
-      <c r="B26" t="s">
-        <v>298</v>
-      </c>
-      <c r="C26" t="s">
-        <v>299</v>
-      </c>
-      <c r="D26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>246</v>
-      </c>
-      <c r="B27" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" t="s">
-        <v>301</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>247</v>
-      </c>
-      <c r="B28" t="s">
-        <v>302</v>
-      </c>
-      <c r="C28" t="s">
-        <v>303</v>
-      </c>
-      <c r="D28" t="s">
-        <v>125</v>
+      <c r="E21" s="6" t="str">
+        <f>AT指令表!H18</f>
+        <v>AT+Z</v>
+      </c>
+      <c r="F21" t="str">
+        <f>AT指令表!I18</f>
+        <v>//设备重启</v>
       </c>
     </row>
   </sheetData>

</xml_diff>